<commit_message>
Add case summary info
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_esd1_rted.xlsx
+++ b/ams/cases/ieee14/ieee14_esd1_rted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F7402-20DB-8F4B-8023-5F6F8D94CBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DC64A2-42F6-1A42-8CD2-13E22AE5253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="288">
   <si>
     <t>uid</t>
   </si>
@@ -1074,22 +1074,16 @@
     <t>comment2</t>
   </si>
   <si>
-    <t>by Jinning Wang</t>
+    <t>Modified IEEE 14-bus test case</t>
+  </si>
+  <si>
+    <t>with dispath ESD1 model</t>
+  </si>
+  <si>
+    <t>comment3</t>
   </si>
   <si>
     <t>for RTED</t>
-  </si>
-  <si>
-    <t>comment3</t>
-  </si>
-  <si>
-    <t>comment4</t>
-  </si>
-  <si>
-    <t>Modified IEEE 14-bus test case</t>
-  </si>
-  <si>
-    <t>with dispath ESD1 model</t>
   </si>
 </sst>
 </file>
@@ -1576,15 +1570,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04FDB8D-C745-F441-9810-AE382BF552E9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1600,28 +1594,22 @@
       <c r="E1" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="7">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>284</v>
+      <c r="E2" s="9" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>